<commit_message>
refactor: remove redundant function
</commit_message>
<xml_diff>
--- a/assets/materials/10-直料/text.xlsx
+++ b/assets/materials/10-直料/text.xlsx
@@ -671,7 +671,7 @@
         <v>99</v>
       </c>
       <c r="M4" s="4" t="n">
-        <v>393</v>
+        <v>388.8</v>
       </c>
       <c r="N4" s="4" t="inlineStr">
         <is>
@@ -709,7 +709,7 @@
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>393.0 kg</t>
+          <t>388.8 kg</t>
         </is>
       </c>
       <c r="E7" s="7" t="inlineStr">
@@ -736,7 +736,7 @@
     <row r="9">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>生成時間：2025-08-13 14:41:07 | 圖示功能：暫時停用，等 assets/materials 圖片準備好時再實作</t>
+          <t>生成時間：2025-08-13 14:51:08 | 圖示功能：暫時停用，等 assets/materials 圖片準備好時再實作</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: modify graph size and set python verison to 3.13
</commit_message>
<xml_diff>
--- a/assets/materials/10-直料/text.xlsx
+++ b/assets/materials/10-直料/text.xlsx
@@ -218,7 +218,7 @@
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1143000" cy="762000"/>
+    <ext cx="1905000" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -645,7 +645,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="80" customHeight="1">
+    <row r="4" ht="120" customHeight="1">
       <c r="A4" s="4" t="n">
         <v>1</v>
       </c>
@@ -736,7 +736,7 @@
     <row r="9">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>生成時間：2025-08-13 14:51:08 | 圖示功能：暫時停用，等 assets/materials 圖片準備好時再實作</t>
+          <t>生成時間：2025-08-13 15:55:09 | 圖示功能：暫時停用，等 assets/materials 圖片準備好時再實作</t>
         </is>
       </c>
     </row>
@@ -744,9 +744,9 @@
   <autoFilter ref="A2:O9"/>
   <mergeCells count="4">
     <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A9:O9"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A6:O6"/>
-    <mergeCell ref="A9:O9"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape"/>

</xml_diff>